<commit_message>
New release compatible with Django 5
</commit_message>
<xml_diff>
--- a/tests/imports/exported.xlsx
+++ b/tests/imports/exported.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t xml:space="preserve">dm3_UzHjrHsFGX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dm3_rewyi</t>
   </si>
 </sst>
 </file>
@@ -187,8 +190,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -220,77 +227,77 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="0" t="s">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="0" t="s">
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="A2" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>403</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G2" s="1" t="n">
+      <c r="G2" s="2" t="n">
         <v>43796</v>
       </c>
-      <c r="I2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="J2" s="2" t="n">
+      <c r="I2" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="J2" s="3" t="n">
         <v>44151.1192447344</v>
       </c>
-      <c r="K2" s="0" t="s">
+      <c r="K2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -306,216 +313,219 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="K15" activeCellId="0" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.31"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="B2" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E2" s="0" t="n">
+      <c r="D2" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="n">
         <v>322</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B3" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C3" s="0" t="s">
+      <c r="B3" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="E3" s="0" t="n">
+      <c r="D3" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="n">
         <v>883</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="0" t="n">
+      <c r="C6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="E4" s="0" t="n">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>19</v>
-      </c>
-      <c r="C5" s="0" t="s">
+      <c r="E6" s="1" t="n">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="D5" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="E5" s="0" t="n">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>26</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="E6" s="0" t="n">
-        <v>815</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C7" s="0" t="s">
+      <c r="D10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="D7" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B8" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="E8" s="0" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="B9" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>14</v>
-      </c>
-      <c r="B10" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="E10" s="0" t="n">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="C11" s="0" t="s">
+      <c r="B12" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="D11" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="E11" s="0" t="n">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="B12" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="E12" s="0" t="n">
+      <c r="D12" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E12" s="1" t="n">
         <v>197</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -528,62 +538,73 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="H18" activeCellId="0" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C2" s="0" t="n">
+      <c r="A2" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="n">
         <v>94</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C3" s="0" t="n">
+      <c r="A3" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="n">
         <v>326</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" s="0" t="n">
+      <c r="B4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="n">
         <v>422</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -596,74 +617,88 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="A2" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>688</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C3" s="0" t="s">
+      <c r="A3" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>244</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>13</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" s="0" t="s">
+      <c r="A4" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>31</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Added fix for max length of tab names
</commit_message>
<xml_diff>
--- a/tests/imports/exported.xlsx
+++ b/tests/imports/exported.xlsx
@@ -9,7 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="app1.demomodel1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="app1.demomodel4" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="app1.verylongnamemodeldemomodel" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="app1.demomodel2" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="app1.demomodel3" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
@@ -190,20 +190,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -220,7 +224,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -306,7 +310,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -318,7 +322,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="4" width="24.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -534,7 +538,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -591,13 +595,13 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C5" s="0" t="n">
+      <c r="B5" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4" t="n">
         <v>95</v>
       </c>
     </row>
@@ -613,7 +617,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -682,16 +686,16 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C5" s="0" t="s">
+      <c r="A5" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="4" t="n">
         <v>78</v>
       </c>
     </row>

</xml_diff>